<commit_message>
spring boot 2 pocs, read me
</commit_message>
<xml_diff>
--- a/spring-boot-2/pocs.xlsx
+++ b/spring-boot-2/pocs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E123EF3E-088E-4221-BD4C-FABADB62C5E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B0904-83E5-47BF-A8CE-4EC3B1912C80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>data jpa mysql</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>Refer definitions/spring/boot/boot-2/pics/integration-testing.jpg</t>
+  </si>
+  <si>
+    <t>file upload</t>
+  </si>
+  <si>
+    <t>spring boot dev tools</t>
+  </si>
+  <si>
+    <t>injecting custom properties</t>
+  </si>
+  <si>
+    <t>custom properties with configuraton file</t>
+  </si>
+  <si>
+    <t>spring boot 2 activemq</t>
   </si>
 </sst>
 </file>
@@ -572,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,6 +798,31 @@
         <v>40</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
read properties file outside jar - references
</commit_message>
<xml_diff>
--- a/spring-boot-2/pocs.xlsx
+++ b/spring-boot-2/pocs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B0904-83E5-47BF-A8CE-4EC3B1912C80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32937A23-C308-4C91-A95F-81D171A79CA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
-  <si>
-    <t>data jpa mysql</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>kafka</t>
   </si>
@@ -47,9 +44,6 @@
     <t>google pub sub integration</t>
   </si>
   <si>
-    <t>validation in spring boot</t>
-  </si>
-  <si>
     <t>APIs - Get, POST, PUT, Patch, Delete</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>multi module project</t>
   </si>
   <si>
-    <t>actuator</t>
-  </si>
-  <si>
     <t>mysql-data-jpa</t>
   </si>
   <si>
@@ -102,12 +93,6 @@
   </si>
   <si>
     <t>circle ci integration</t>
-  </si>
-  <si>
-    <t>global exception handling with hibernate bean validation</t>
-  </si>
-  <si>
-    <t>data-jpa calling stored procedures</t>
   </si>
   <si>
     <t>data-jpa calling mysql functions</t>
@@ -202,12 +187,18 @@
   <si>
     <t>spring boot 2 activemq</t>
   </si>
+  <si>
+    <t>https://www.journaldev.com/18141/spring-boot-redis-cache
+https://dzone.com/articles/implementation-of-redis-in-micro-servicespring-boo
+https://www.devglan.com/spring-boot/spring-boot-redis-cache
+https://www.concretepage.com/spring-boot/spring-boot-redis-cache</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +210,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,16 +240,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A2:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,232 +603,213 @@
     <col min="2" max="2" width="82.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" display="https://www.journaldev.com/18141/spring-boot-redis-cache_x000a_" xr:uid="{E3158EE8-60BE-478D-A4E5-8E68C471CE74}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>